<commit_message>
Final changes for last pieces of feedback provided.
</commit_message>
<xml_diff>
--- a/v1.5/Release Candidate/OpenSAMM_Assessment_Toolbox_v1.5-Example_RC1.xlsx
+++ b/v1.5/Release Candidate/OpenSAMM_Assessment_Toolbox_v1.5-Example_RC1.xlsx
@@ -4848,7 +4848,7 @@
                   <c:v>1.483333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.05</c:v>
@@ -5396,7 +5396,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -5414,7 +5416,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -5432,7 +5436,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -5608,7 +5614,7 @@
                   <c:v>1.483333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.05</c:v>
@@ -5721,7 +5727,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -5739,7 +5747,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -5757,7 +5767,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -6046,7 +6058,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -6064,7 +6078,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -6082,7 +6098,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -6371,7 +6389,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -6389,7 +6409,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -6407,7 +6429,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -7022,10 +7046,10 @@
                   <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
-                  <c:v>2.0</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8239,7 +8263,7 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1.516666666666667</c:v>
@@ -8684,7 +8708,7 @@
                   <c:v>1.483333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.05</c:v>
@@ -8948,7 +8972,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8966,7 +8992,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8984,7 +9012,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9275,7 +9305,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9293,7 +9325,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9311,7 +9345,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9600,7 +9636,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9618,7 +9656,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9636,7 +9676,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9788,7 +9830,7 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1.516666666666667</c:v>
@@ -9925,7 +9967,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9943,7 +9987,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9961,7 +10007,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -10740,7 +10788,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.2</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5</c:v>
@@ -14277,7 +14325,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14454,7 +14502,7 @@
   <dimension ref="A1:Z447"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F2" sqref="F1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -15149,13 +15197,13 @@
       </c>
       <c r="D23" s="249"/>
       <c r="E23" s="22" t="s">
-        <v>424</v>
+        <v>493</v>
       </c>
       <c r="F23" s="18">
         <v>2</v>
       </c>
       <c r="G23" s="18">
-        <f>IFERROR(VLOOKUP(E23,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E23,AnswerCTBL,2,FALSE),0)</f>
         <v>0.2</v>
       </c>
       <c r="H23" s="109"/>
@@ -15308,13 +15356,13 @@
       </c>
       <c r="D28" s="249"/>
       <c r="E28" s="22" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="F28" s="18">
         <v>3</v>
       </c>
       <c r="G28" s="18">
-        <f>IFERROR(VLOOKUP(E28,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E28,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="H28" s="109"/>
@@ -15817,13 +15865,13 @@
       </c>
       <c r="D44" s="271"/>
       <c r="E44" s="22" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="F44" s="18">
         <v>6</v>
       </c>
       <c r="G44" s="18">
-        <f>IFERROR(VLOOKUP(E44,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E44,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="H44" s="109"/>
@@ -16394,13 +16442,13 @@
       </c>
       <c r="D62" s="255"/>
       <c r="E62" s="5" t="s">
-        <v>424</v>
+        <v>493</v>
       </c>
       <c r="F62" s="18">
         <v>9</v>
       </c>
       <c r="G62" s="18">
-        <f>IFERROR(VLOOKUP(E62,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E62,AnswerCTBL,2,FALSE),0)</f>
         <v>0.2</v>
       </c>
       <c r="H62" s="108">
@@ -16410,7 +16458,7 @@
       <c r="I62" s="257"/>
       <c r="J62" s="250">
         <f>SUM(H62,H73,H89)</f>
-        <v>1.2</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="K62" s="1"/>
       <c r="L62" s="141"/>
@@ -16758,7 +16806,7 @@
       </c>
       <c r="H73" s="109">
         <f>IFERROR(AVERAGE(G73,G81),0)</f>
-        <v>0.5</v>
+        <v>0.35</v>
       </c>
       <c r="I73" s="309"/>
       <c r="J73" s="11"/>
@@ -17002,14 +17050,14 @@
       </c>
       <c r="D81" s="249"/>
       <c r="E81" s="22" t="s">
-        <v>430</v>
+        <v>493</v>
       </c>
       <c r="F81" s="18">
         <v>12</v>
       </c>
       <c r="G81" s="18">
-        <f>IFERROR(VLOOKUP(E81,AnswerETBL,2,FALSE),0)</f>
-        <v>0.5</v>
+        <f>IFERROR(VLOOKUP(E81,AnswerCTBL,2,FALSE),0)</f>
+        <v>0.2</v>
       </c>
       <c r="H81" s="109"/>
       <c r="I81" s="257"/>
@@ -17263,7 +17311,7 @@
       </c>
       <c r="H89" s="109">
         <f>IFERROR(AVERAGE(G89,G94),0)</f>
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="I89" s="257"/>
       <c r="J89" s="11"/>
@@ -17414,14 +17462,14 @@
       </c>
       <c r="D94" s="249"/>
       <c r="E94" s="22" t="s">
-        <v>430</v>
+        <v>442</v>
       </c>
       <c r="F94" s="18">
         <v>14</v>
       </c>
       <c r="G94" s="18">
-        <f>IFERROR(VLOOKUP(E94,AnswerETBL,2,FALSE),0)</f>
-        <v>0.5</v>
+        <f>IFERROR(VLOOKUP(E94,AnswerGTBL,2,FALSE),0)</f>
+        <v>0.2</v>
       </c>
       <c r="H94" s="109"/>
       <c r="I94" s="257"/>
@@ -19452,13 +19500,13 @@
       </c>
       <c r="D158" s="249"/>
       <c r="E158" s="22" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="F158" s="18">
         <v>5</v>
       </c>
       <c r="G158" s="18">
-        <f>IFERROR(VLOOKUP(E158,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E158,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="H158" s="109"/>
@@ -22641,13 +22689,13 @@
       </c>
       <c r="D259" s="249"/>
       <c r="E259" s="22" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="F259" s="18">
         <v>4</v>
       </c>
       <c r="G259" s="18">
-        <f>IFERROR(VLOOKUP(E259,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E259,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="H259" s="109"/>
@@ -23525,13 +23573,13 @@
       </c>
       <c r="D287" s="255"/>
       <c r="E287" s="5" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
       <c r="F287" s="18">
         <v>9</v>
       </c>
       <c r="G287" s="18">
-        <f>IFERROR(VLOOKUP(E287,AnswerGTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E287,AnswerFTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="H287" s="109">
@@ -24384,13 +24432,13 @@
       </c>
       <c r="D314" s="249"/>
       <c r="E314" s="22" t="s">
-        <v>424</v>
+        <v>493</v>
       </c>
       <c r="F314" s="18">
         <v>15</v>
       </c>
       <c r="G314" s="18">
-        <f>IFERROR(VLOOKUP(E314,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E314,AnswerCTBL,2,FALSE),0)</f>
         <v>0.2</v>
       </c>
       <c r="H314" s="109"/>
@@ -25139,13 +25187,13 @@
       </c>
       <c r="D338" s="255"/>
       <c r="E338" s="5" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="F338" s="18">
         <v>1</v>
       </c>
       <c r="G338" s="18">
-        <f>IFERROR(VLOOKUP(E338,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E338,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="H338" s="109">
@@ -25395,13 +25443,13 @@
       </c>
       <c r="D346" s="249"/>
       <c r="E346" s="22" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="F346" s="18">
         <v>3</v>
       </c>
       <c r="G346" s="18">
-        <f>IFERROR(VLOOKUP(E346,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E346,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="H346" s="109"/>
@@ -25832,13 +25880,13 @@
       </c>
       <c r="D360" s="249"/>
       <c r="E360" s="22" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="F360" s="18">
         <v>5</v>
       </c>
       <c r="G360" s="18">
-        <f>IFERROR(VLOOKUP(E360,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E360,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="H360" s="109"/>
@@ -28873,10 +28921,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E346 E360 M28:P28 E158 E314 E338 E62 E44 E28 E23 E259 M23:P23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M23:P23 M28:P28">
       <formula1>AnswerB</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E150 E138 E162 E166 E173 E185 E192 E196 E211 E154 E239 E247 E254 E265 E281 E291 E304 E309 E324 E329 E364 E370 E382 E392 E411 E417 E424 E431 E144 E118 E111 E41 E89 E35 E48 E105 E376 E320 E229">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E150 E138 E162 E166 E173 E185 E192 E196 E211 E154 E239 E247 E254 E265 E281 E291 E304 E309 E324 E329 E364 E370 E382 E392 E411 E417 E424 E431 E144 E118 E111 E41 E89 E35 E48 E105 E376 E320 E229 E81 E23 E28 E44 E62 E158 E259 E314 E338 E346 E360">
       <formula1>AnswerC</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E18 E342 M18:P18">
@@ -28885,13 +28933,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E56 E199 E130 E100 E233 E439">
       <formula1>AnswerD</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E65 E81 E94 E443">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E65 E443">
       <formula1>AnswerE</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E73 E124 E206 E223 E179 E400 E270 E299 E332">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E73 E124 E206 E223 E179 E400 E270 E299 E332 E287">
       <formula1>AnswerF</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E216 E404 E350 E277 E287 E296 E387">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E216 E404 E350 E277 E387 E296 E94">
       <formula1>AnswerG</formula1>
     </dataValidation>
   </dataValidations>
@@ -29273,7 +29321,7 @@
       </c>
       <c r="J14" s="107">
         <f>AVERAGE(C14:C16)</f>
-        <v>1.2444444444444445</v>
+        <v>1.1444444444444446</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -29286,7 +29334,7 @@
       </c>
       <c r="V14" s="107">
         <f>Interview!$J$62</f>
-        <v>1.2</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="W14" s="107">
         <v>0</v>
@@ -29307,7 +29355,7 @@
       </c>
       <c r="C15" s="107">
         <f>Interview!$J$62</f>
-        <v>1.2</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="D15" s="107">
         <f>Interview!H62</f>
@@ -29315,11 +29363,11 @@
       </c>
       <c r="E15" s="107">
         <f>Interview!H73</f>
-        <v>0.5</v>
+        <v>0.35</v>
       </c>
       <c r="F15" s="107">
         <f>Interview!H89</f>
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="G15" s="6">
         <f t="shared" si="0"/>
@@ -30190,7 +30238,7 @@
       </c>
       <c r="J34" s="107">
         <f>AVERAGE(C38:C40)</f>
-        <v>1.8388888888888888</v>
+        <v>1.9222222222222223</v>
       </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -30431,7 +30479,7 @@
       </c>
       <c r="X38" s="107">
         <f>'Roadmap Chart'!I19</f>
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="Y38" s="107">
         <v>0</v>
@@ -30446,7 +30494,7 @@
       </c>
       <c r="C39" s="107">
         <f>Roadmap!Y88</f>
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="D39" s="107">
         <f>Roadmap!X88</f>
@@ -30454,7 +30502,7 @@
       </c>
       <c r="E39" s="107">
         <f>Roadmap!X91</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F39" s="107">
         <f>Roadmap!X94</f>
@@ -30462,7 +30510,7 @@
       </c>
       <c r="G39" s="6">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="139"/>
@@ -32308,7 +32356,7 @@
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
-      <selection pane="topRight" activeCell="E6" sqref="E6"/>
+      <selection pane="topRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -33034,49 +33082,49 @@
       <c r="D21" s="383"/>
       <c r="E21" s="30" t="str">
         <f>Interview!E23</f>
-        <v>Yes, some of them are aware</v>
+        <v>Yes, a small percentage are/do</v>
       </c>
       <c r="F21" s="156">
         <v>2</v>
       </c>
       <c r="G21" s="156">
-        <f>IFERROR(VLOOKUP(E21,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E21,AnswerCTBL,2,FALSE),0)</f>
         <v>0.2</v>
       </c>
       <c r="H21" s="201"/>
       <c r="I21" s="381"/>
       <c r="J21" s="177" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="K21" s="156">
-        <f>IFERROR(VLOOKUP(J21,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(J21,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="L21" s="158"/>
       <c r="M21" s="373"/>
       <c r="N21" s="177" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="O21" s="156">
-        <f>IFERROR(VLOOKUP(N21,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(N21,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="P21" s="158"/>
       <c r="Q21" s="373"/>
       <c r="R21" s="177" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="S21" s="156">
-        <f>IFERROR(VLOOKUP(R21,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(R21,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="T21" s="158"/>
       <c r="U21" s="373"/>
       <c r="V21" s="177" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="W21" s="156">
-        <f>IFERROR(VLOOKUP(V21,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(V21,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="X21" s="158"/>
@@ -33094,49 +33142,49 @@
       <c r="D22" s="385"/>
       <c r="E22" s="30" t="str">
         <f>Interview!E28</f>
-        <v>Yes, most of them are aware</v>
+        <v>Yes, the majority of them are/do</v>
       </c>
       <c r="F22" s="18">
         <v>3</v>
       </c>
       <c r="G22" s="18">
-        <f>IFERROR(VLOOKUP(E22,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E22,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="H22" s="202"/>
       <c r="I22" s="212"/>
       <c r="J22" s="177" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="K22" s="18">
-        <f>IFERROR(VLOOKUP(J22,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(J22,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="L22" s="109"/>
       <c r="M22" s="373"/>
       <c r="N22" s="177" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="O22" s="18">
-        <f>IFERROR(VLOOKUP(N22,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(N22,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="P22" s="109"/>
       <c r="Q22" s="373"/>
       <c r="R22" s="177" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="S22" s="18">
-        <f>IFERROR(VLOOKUP(R22,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(R22,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="T22" s="109"/>
       <c r="U22" s="373"/>
       <c r="V22" s="177" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="W22" s="18">
-        <f>IFERROR(VLOOKUP(V22,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(V22,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="X22" s="109"/>
@@ -33317,49 +33365,49 @@
       <c r="D26" s="392"/>
       <c r="E26" s="30" t="str">
         <f>Interview!E44</f>
-        <v>Yes, approx. half of them are aware</v>
+        <v>Yes, at least half of them are/do</v>
       </c>
       <c r="F26" s="18">
         <v>6</v>
       </c>
       <c r="G26" s="18">
-        <f>IFERROR(VLOOKUP(E26,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E26,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="H26" s="202"/>
       <c r="I26" s="212"/>
       <c r="J26" s="177" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="K26" s="18">
-        <f>IFERROR(VLOOKUP(J26,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(J26,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="L26" s="109"/>
       <c r="M26" s="180"/>
       <c r="N26" s="177" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="O26" s="18">
-        <f>IFERROR(VLOOKUP(N26,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(N26,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="P26" s="109"/>
       <c r="Q26" s="180"/>
       <c r="R26" s="177" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="S26" s="18">
-        <f>IFERROR(VLOOKUP(R26,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(R26,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="T26" s="109"/>
       <c r="U26" s="180"/>
       <c r="V26" s="177" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="W26" s="18">
-        <f>IFERROR(VLOOKUP(V26,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(V26,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="X26" s="109"/>
@@ -33590,13 +33638,13 @@
       <c r="D31" s="390"/>
       <c r="E31" s="30" t="str">
         <f>Interview!E62</f>
-        <v>Yes, some of them are aware</v>
+        <v>Yes, a small percentage are/do</v>
       </c>
       <c r="F31" s="156">
         <v>9</v>
       </c>
       <c r="G31" s="156">
-        <f>IFERROR(VLOOKUP(E31,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E31,AnswerCTBL,2,FALSE),0)</f>
         <v>0.2</v>
       </c>
       <c r="H31" s="204">
@@ -33605,13 +33653,13 @@
       </c>
       <c r="I31" s="380">
         <f>SUM(H31,H34,H37)</f>
-        <v>1.2</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="J31" s="177" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="K31" s="156">
-        <f>IFERROR(VLOOKUP(J31,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(J31,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="L31" s="142">
@@ -33623,10 +33671,10 @@
         <v>1.5</v>
       </c>
       <c r="N31" s="177" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="O31" s="156">
-        <f>IFERROR(VLOOKUP(N31,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(N31,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="P31" s="142">
@@ -33638,10 +33686,10 @@
         <v>1.75</v>
       </c>
       <c r="R31" s="177" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="S31" s="156">
-        <f>IFERROR(VLOOKUP(R31,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(R31,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="T31" s="142">
@@ -33653,10 +33701,10 @@
         <v>2</v>
       </c>
       <c r="V31" s="177" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="W31" s="156">
-        <f>IFERROR(VLOOKUP(V31,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(V31,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="X31" s="142">
@@ -33779,7 +33827,7 @@
       </c>
       <c r="H34" s="201">
         <f>IFERROR(AVERAGE(G34,G35),0)</f>
-        <v>0.5</v>
+        <v>0.35</v>
       </c>
       <c r="I34" s="212"/>
       <c r="J34" s="177" t="s">
@@ -33843,49 +33891,49 @@
       <c r="D35" s="385"/>
       <c r="E35" s="30" t="str">
         <f>Interview!E81</f>
-        <v>Yes, but on an adhoc basis</v>
+        <v>Yes, a small percentage are/do</v>
       </c>
       <c r="F35" s="18">
         <v>12</v>
       </c>
       <c r="G35" s="18">
-        <f>IFERROR(VLOOKUP(E35,AnswerETBL,2,FALSE),0)</f>
-        <v>0.5</v>
+        <f>IFERROR(VLOOKUP(E35,AnswerCTBL,2,FALSE),0)</f>
+        <v>0.2</v>
       </c>
       <c r="H35" s="202"/>
       <c r="I35" s="212"/>
       <c r="J35" s="177" t="s">
-        <v>430</v>
+        <v>494</v>
       </c>
       <c r="K35" s="18">
-        <f>IFERROR(VLOOKUP(J35,AnswerETBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(J35,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="L35" s="109"/>
       <c r="M35" s="180"/>
       <c r="N35" s="177" t="s">
-        <v>430</v>
+        <v>494</v>
       </c>
       <c r="O35" s="18">
-        <f>IFERROR(VLOOKUP(N35,AnswerETBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(N35,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="P35" s="109"/>
       <c r="Q35" s="180"/>
       <c r="R35" s="177" t="s">
-        <v>369</v>
+        <v>495</v>
       </c>
       <c r="S35" s="18">
-        <f>IFERROR(VLOOKUP(R35,AnswerETBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(R35,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="T35" s="109"/>
       <c r="U35" s="180"/>
       <c r="V35" s="177" t="s">
-        <v>369</v>
+        <v>495</v>
       </c>
       <c r="W35" s="18">
-        <f>IFERROR(VLOOKUP(V35,AnswerETBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(V35,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="X35" s="109"/>
@@ -33942,7 +33990,7 @@
       </c>
       <c r="H37" s="201">
         <f>IFERROR(AVERAGE(G37,G38),0)</f>
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="I37" s="212"/>
       <c r="J37" s="176" t="s">
@@ -34006,49 +34054,49 @@
       <c r="D38" s="385"/>
       <c r="E38" s="30" t="str">
         <f>Interview!E94</f>
-        <v>Yes, but on an adhoc basis</v>
+        <v>Yes, localized to business areas</v>
       </c>
       <c r="F38" s="18">
         <v>14</v>
       </c>
       <c r="G38" s="18">
-        <f>IFERROR(VLOOKUP(E38,AnswerETBL,2,FALSE),0)</f>
-        <v>0.5</v>
+        <f>IFERROR(VLOOKUP(E38,AnswerGTBL,2,FALSE),0)</f>
+        <v>0.2</v>
       </c>
       <c r="H38" s="202"/>
       <c r="I38" s="212"/>
       <c r="J38" s="177" t="s">
-        <v>430</v>
+        <v>444</v>
       </c>
       <c r="K38" s="18">
-        <f>IFERROR(VLOOKUP(J38,AnswerETBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(J38,AnswerGTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="L38" s="109"/>
       <c r="M38" s="180"/>
       <c r="N38" s="177" t="s">
-        <v>430</v>
+        <v>444</v>
       </c>
       <c r="O38" s="18">
-        <f>IFERROR(VLOOKUP(N38,AnswerETBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(N38,AnswerGTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="P38" s="109"/>
       <c r="Q38" s="180"/>
       <c r="R38" s="177" t="s">
-        <v>430</v>
+        <v>444</v>
       </c>
       <c r="S38" s="18">
-        <f>IFERROR(VLOOKUP(R38,AnswerETBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(R38,AnswerGTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="T38" s="109"/>
       <c r="U38" s="180"/>
       <c r="V38" s="177" t="s">
-        <v>369</v>
+        <v>443</v>
       </c>
       <c r="W38" s="18">
-        <f>IFERROR(VLOOKUP(V38,AnswerETBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(V38,AnswerGTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="X38" s="109"/>
@@ -34982,49 +35030,49 @@
       <c r="D55" s="385"/>
       <c r="E55" s="30" t="str">
         <f>Interview!E158</f>
-        <v>Yes, approx. half of them are aware</v>
+        <v>Yes, at least half of them are/do</v>
       </c>
       <c r="F55" s="18">
         <v>5</v>
       </c>
       <c r="G55" s="18">
-        <f>IFERROR(VLOOKUP(E55,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E55,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="H55" s="166"/>
       <c r="I55" s="212"/>
       <c r="J55" s="177" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="K55" s="18">
-        <f>IFERROR(VLOOKUP(J55,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(J55,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="L55" s="109"/>
       <c r="M55" s="180"/>
       <c r="N55" s="177" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="O55" s="18">
-        <f>IFERROR(VLOOKUP(N55,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(N55,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="P55" s="109"/>
       <c r="Q55" s="180"/>
       <c r="R55" s="177" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="S55" s="18">
-        <f>IFERROR(VLOOKUP(R55,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(R55,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="T55" s="109"/>
       <c r="U55" s="180"/>
       <c r="V55" s="177" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="W55" s="18">
-        <f>IFERROR(VLOOKUP(V55,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(V55,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="X55" s="109"/>
@@ -36572,49 +36620,49 @@
       <c r="D83" s="385"/>
       <c r="E83" s="30" t="str">
         <f>Interview!E259</f>
-        <v>Yes, approx. half of them are aware</v>
+        <v>Yes, at least half of them are/do</v>
       </c>
       <c r="F83" s="18">
         <v>4</v>
       </c>
       <c r="G83" s="18">
-        <f>IFERROR(VLOOKUP(E83,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E83,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="H83" s="166"/>
       <c r="I83" s="212"/>
       <c r="J83" s="177" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="K83" s="18">
-        <f>IFERROR(VLOOKUP(J83,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(J83,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="L83" s="109"/>
       <c r="M83" s="180"/>
       <c r="N83" s="177" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="O83" s="18">
-        <f>IFERROR(VLOOKUP(N83,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(N83,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="P83" s="109"/>
       <c r="Q83" s="180"/>
       <c r="R83" s="177" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="S83" s="18">
-        <f>IFERROR(VLOOKUP(R83,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(R83,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="T83" s="109"/>
       <c r="U83" s="180"/>
       <c r="V83" s="177" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="W83" s="18">
-        <f>IFERROR(VLOOKUP(V83,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(V83,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="X83" s="109"/>
@@ -36916,7 +36964,7 @@
       </c>
       <c r="Y88" s="367">
         <f>SUM(X88,X91,X94)</f>
-        <v>2</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="89" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -37016,13 +37064,13 @@
       <c r="D91" s="390"/>
       <c r="E91" s="30" t="str">
         <f>Interview!E287</f>
-        <v>Yes, across the organization</v>
+        <v>Yes, there is a standard set</v>
       </c>
       <c r="F91" s="18">
         <v>9</v>
       </c>
       <c r="G91" s="18">
-        <f>IFERROR(VLOOKUP(E91,AnswerGTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E91,AnswerFTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="H91" s="166">
@@ -37031,10 +37079,10 @@
       </c>
       <c r="I91" s="212"/>
       <c r="J91" s="176" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
       <c r="K91" s="18">
-        <f>IFERROR(VLOOKUP(J91,AnswerGTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(J91,AnswerFTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="L91" s="109">
@@ -37043,10 +37091,10 @@
       </c>
       <c r="M91" s="180"/>
       <c r="N91" s="176" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
       <c r="O91" s="18">
-        <f>IFERROR(VLOOKUP(N91,AnswerGTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(N91,AnswerFTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="P91" s="109">
@@ -37055,10 +37103,10 @@
       </c>
       <c r="Q91" s="180"/>
       <c r="R91" s="176" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
       <c r="S91" s="18">
-        <f>IFERROR(VLOOKUP(R91,AnswerGTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(R91,AnswerFTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="T91" s="109">
@@ -37067,15 +37115,15 @@
       </c>
       <c r="U91" s="180"/>
       <c r="V91" s="176" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
       <c r="W91" s="18">
-        <f>IFERROR(VLOOKUP(V91,AnswerGTBL,2,FALSE),0)</f>
-        <v>0.5</v>
+        <f>IFERROR(VLOOKUP(V91,AnswerFTBL,2,FALSE),0)</f>
+        <v>1</v>
       </c>
       <c r="X91" s="109">
         <f>IFERROR(AVERAGE(W91,W92),0)</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="Y91" s="180"/>
     </row>
@@ -37504,49 +37552,49 @@
       <c r="D99" s="385"/>
       <c r="E99" s="30" t="str">
         <f>Interview!E314</f>
-        <v>Yes, some of them are aware</v>
+        <v>Yes, a small percentage are/do</v>
       </c>
       <c r="F99" s="18">
         <v>15</v>
       </c>
       <c r="G99" s="18">
-        <f>IFERROR(VLOOKUP(E99,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E99,AnswerCTBL,2,FALSE),0)</f>
         <v>0.2</v>
       </c>
       <c r="H99" s="166"/>
       <c r="I99" s="212"/>
       <c r="J99" s="177" t="s">
-        <v>424</v>
+        <v>493</v>
       </c>
       <c r="K99" s="18">
-        <f>IFERROR(VLOOKUP(J99,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(J99,AnswerCTBL,2,FALSE),0)</f>
         <v>0.2</v>
       </c>
       <c r="L99" s="109"/>
       <c r="M99" s="180"/>
       <c r="N99" s="177" t="s">
-        <v>424</v>
+        <v>493</v>
       </c>
       <c r="O99" s="18">
-        <f>IFERROR(VLOOKUP(N99,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(N99,AnswerCTBL,2,FALSE),0)</f>
         <v>0.2</v>
       </c>
       <c r="P99" s="109"/>
       <c r="Q99" s="180"/>
       <c r="R99" s="177" t="s">
-        <v>424</v>
+        <v>493</v>
       </c>
       <c r="S99" s="18">
-        <f>IFERROR(VLOOKUP(R99,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(R99,AnswerCTBL,2,FALSE),0)</f>
         <v>0.2</v>
       </c>
       <c r="T99" s="109"/>
       <c r="U99" s="180"/>
       <c r="V99" s="177" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="W99" s="18">
-        <f>IFERROR(VLOOKUP(V99,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(V99,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="X99" s="109"/>
@@ -37972,13 +38020,13 @@
       <c r="D108" s="390"/>
       <c r="E108" s="29" t="str">
         <f>Interview!E338</f>
-        <v>Yes, most of them are aware</v>
+        <v>Yes, the majority of them are/do</v>
       </c>
       <c r="F108" s="152">
         <v>1</v>
       </c>
       <c r="G108" s="152">
-        <f>IFERROR(VLOOKUP(E108,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E108,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="H108" s="208">
@@ -37990,10 +38038,10 @@
         <v>1.9333333333333336</v>
       </c>
       <c r="J108" s="176" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="K108" s="18">
-        <f>IFERROR(VLOOKUP(J108,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(J108,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="L108" s="109">
@@ -38005,10 +38053,10 @@
         <v>1.9333333333333336</v>
       </c>
       <c r="N108" s="176" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="O108" s="18">
-        <f>IFERROR(VLOOKUP(N108,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(N108,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="P108" s="109">
@@ -38020,10 +38068,10 @@
         <v>2.0833333333333335</v>
       </c>
       <c r="R108" s="176" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="S108" s="18">
-        <f>IFERROR(VLOOKUP(R108,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(R108,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="T108" s="109">
@@ -38035,10 +38083,10 @@
         <v>2.0833333333333335</v>
       </c>
       <c r="V108" s="176" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="W108" s="18">
-        <f>IFERROR(VLOOKUP(V108,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(V108,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="X108" s="109">
@@ -38118,49 +38166,49 @@
       <c r="D110" s="385"/>
       <c r="E110" s="30" t="str">
         <f>Interview!E346</f>
-        <v>Yes, most of them are aware</v>
+        <v>Yes, the majority of them are/do</v>
       </c>
       <c r="F110" s="18">
         <v>3</v>
       </c>
       <c r="G110" s="18">
-        <f>IFERROR(VLOOKUP(E110,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E110,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="H110" s="202"/>
       <c r="I110" s="212"/>
       <c r="J110" s="177" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="K110" s="18">
-        <f>IFERROR(VLOOKUP(J110,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(J110,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="L110" s="109"/>
       <c r="M110" s="180"/>
       <c r="N110" s="177" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="O110" s="18">
-        <f>IFERROR(VLOOKUP(N110,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(N110,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="P110" s="109"/>
       <c r="Q110" s="180"/>
       <c r="R110" s="177" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="S110" s="18">
-        <f>IFERROR(VLOOKUP(R110,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(R110,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="T110" s="109"/>
       <c r="U110" s="180"/>
       <c r="V110" s="177" t="s">
-        <v>425</v>
+        <v>495</v>
       </c>
       <c r="W110" s="18">
-        <f>IFERROR(VLOOKUP(V110,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(V110,AnswerCTBL,2,FALSE),0)</f>
         <v>1</v>
       </c>
       <c r="X110" s="109"/>
@@ -38278,49 +38326,49 @@
       <c r="D113" s="385"/>
       <c r="E113" s="30" t="str">
         <f>Interview!E360</f>
-        <v>Yes, approx. half of them are aware</v>
+        <v>Yes, at least half of them are/do</v>
       </c>
       <c r="F113" s="18">
         <v>5</v>
       </c>
       <c r="G113" s="18">
-        <f>IFERROR(VLOOKUP(E113,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(E113,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="H113" s="202"/>
       <c r="I113" s="212"/>
       <c r="J113" s="177" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="K113" s="18">
-        <f>IFERROR(VLOOKUP(J113,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(J113,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="L113" s="109"/>
       <c r="M113" s="180"/>
       <c r="N113" s="177" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="O113" s="18">
-        <f>IFERROR(VLOOKUP(N113,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(N113,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="P113" s="109"/>
       <c r="Q113" s="180"/>
       <c r="R113" s="177" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="S113" s="18">
-        <f>IFERROR(VLOOKUP(R113,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(R113,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="T113" s="109"/>
       <c r="U113" s="180"/>
       <c r="V113" s="177" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="W113" s="18">
-        <f>IFERROR(VLOOKUP(V113,AnswerBTBL,2,FALSE),0)</f>
+        <f>IFERROR(VLOOKUP(V113,AnswerCTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
       <c r="X113" s="109"/>
@@ -39813,14 +39861,14 @@
       <formula>W20&lt;S20</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R125 V72 R72 N125 N121 V125 J94 N112 R88 V91 R94 N91 J72 V121 V94 J88 J91 N94 V88 R112 J112 V112 J121 J125 N72 R121 R91 N88">
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R125 V72 R72 N125 N121 V125 J94 N112 R88 N88 R94 R121 J72 V121 V94 J88 N72 N94 V88 R112 J112 V112 J121 J125 J38 N38 R38 V38">
       <formula1>AnswerG</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V105 V46 R73 N105 J105 V95 R105 R46 J34 V34 R69 J61 J69 J73 J46 V69 N34 V61 R61 N61 N69 N73 N46 V73 R34 R95 J124 N124 R124 V124 J86 N86 R86 V86 J95 N95">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V105 V46 R73 N105 J105 V95 R105 R46 J34 V34 R69 J61 J69 J73 J46 V69 N34 V61 R61 N61 N69 N73 N46 V73 R34 R95 J124 N124 R124 V124 J86 N86 R86 V86 J95 N95 J91 N91 R91 V91">
       <formula1>AnswerF</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V134 J32 N32 R32 V32 J35 J38 N35 N38 R35 R38 V35 V38 R134 N134 J134">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V134 J32 N32 R32 V32 J134 N134 R134">
       <formula1>AnswerE</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V133 J133 N133 R133 J29 J67 J47 J40 N29 N67 N47 N40 R29 R67 R47 R40 V29 V67 V47 V40 V76 J76 N76 R76">
@@ -39829,11 +39877,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V20 V109 J20 J109 N20 N109 R20 R109">
       <formula1>AnswerA</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R101 J101 N41 V118 R118 N118 V54 J75 V51 R51 N51 J51 V41 R41 J41 V43:V44 V130:V131 V127:V128 V122 V119 V115:V116 J118 V101 N75 R75 V75 J53 J50 J57:J58 J60 J63:J64 J66 J70 N54 J79:J80 J82 J85 J89 J92 J97:J98 J102 J104 J115:J116 J119 J122 J127:J128 J130:J131 J43:J44 V28 V24:V25 J28 J24:J25 J54 N50 N57:N58 N60 N63:N64 N66 N70 R53 N79:N80 N82 N85 N89 N92 N97:N98 N102 N104 N115:N116 N119 N122 N127:N128 N130:N131 N43:N44 J37 N37 N28 N24:N25 N101 R50 R57:R58 R60 R63:R64 R66 R70 R54 R79:R80 R82 R85 R89 R92 R97:R98 R102 R104 R115:R116 R119 R122 R127:R128 R130:R131 R43:R44 V37 R37 R28 R24:R25 N53 V50 V57:V58 V60 V63:V64 V66 V70 V53 V79:V80 V82 V85 V89 V92 V97:V98 V102 V104">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R101 J101 N41 V118 R118 N118 V54 J75 V51 R51 N51 J51 V41 R41 J41 V43:V44 V130:V131 V127:V128 V122 V119 V115:V116 J118 V101 N75 R75 V75 J53 J50 J57:J58 J60 J63:J64 J66 J70 N54 J79:J80 J82 J85 J89 J92 J97:J98 J102 J104 J115:J116 J119 J122 J127:J128 J130:J131 J43:J44 V28 V24:V25 J28 J24:J25 J54 N50 N57:N58 N60 N63:N64 N66 N70 R53 N79:N80 N82 N85 N89 N92 N97:N98 N102 N104 N115:N116 N119 N122 N127:N128 N130:N131 N43:N44 J37 N37 N28 N24:N25 N101 R50 R57:R58 R60 R63:R64 R66 R70 R54 R79:R80 R82 R85 R89 R92 R97:R98 R102 R104 R115:R116 R119 R122 R127:R128 R130:R131 R43:R44 V37 R37 R28 R24:R25 N53 V50 V57:V58 V60 V63:V64 V66 V70 V53 V79:V80 V82 V85 V89 V92 V97:V98 V102 V104 J35 N35 R35 V35 J21 J22 J26 N21 N22 N26 R21 R22 R26 V21 V22 V26 J31 N31 R31 V31 R55 N55 J55 V55 J83 J99 N83 N99 R83 V83 R99 V99 J108 J110 J113 N108 N110 N113 R108 R110 R113 V108 V110 V113">
       <formula1>AnswerC</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R26 R31 V83 V113 R83 R21:R22 V21:V22 V55 V99 V110 J110 J113 V108 J55 J99 J108 J31 J26 J21:J22 J83 N110 N113 V31 N55 N99 N108 N31 N26 N21:N22 N83 R110 R113 V26 R55 R99 R108">
-      <formula1>AnswerB</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -40204,7 +40249,7 @@
       </c>
       <c r="B13" s="110">
         <f>IF(ISNUMBER(Interview!$J$62),Interview!$J$62,SUM(LEFT(Interview!$J$62),".5"))</f>
-        <v>1.2</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="C13" s="219">
         <f>Roadmap!M31</f>
@@ -40240,7 +40285,7 @@
       </c>
       <c r="K13" s="135">
         <f t="shared" ref="K13:K23" si="0">IFERROR(I13-B13,I13-LEFT(B13,1))</f>
-        <v>1.3</v>
+        <v>1.6</v>
       </c>
       <c r="L13" s="229"/>
       <c r="M13" s="229"/>
@@ -40275,7 +40320,7 @@
       </c>
       <c r="AE13" s="136">
         <f t="shared" ref="AE13:AE23" si="6">B13</f>
-        <v>1.2</v>
+        <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -40715,15 +40760,15 @@
       </c>
       <c r="I19" s="219">
         <f>Roadmap!Y88</f>
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="J19" s="48">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="K19" s="135">
         <f t="shared" si="0"/>
-        <v>0.95000000000000018</v>
+        <v>1.2000000000000002</v>
       </c>
       <c r="L19" s="229"/>
       <c r="M19" s="229"/>
@@ -40742,7 +40787,7 @@
       </c>
       <c r="AA19" s="136">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="AB19" s="136">
         <f t="shared" si="3"/>
@@ -41103,7 +41148,7 @@
       </c>
       <c r="C25" s="136">
         <f>SUM(C12:C23)-SUM(B12:B23)</f>
-        <v>1.0500000000000007</v>
+        <v>1.3500000000000014</v>
       </c>
       <c r="D25" s="136"/>
       <c r="E25" s="136">
@@ -41118,12 +41163,12 @@
       <c r="H25" s="136"/>
       <c r="I25" s="136">
         <f>SUM(I12:I23)-SUM(G12:G23)</f>
-        <v>2.2166666666666686</v>
+        <v>2.4666666666666686</v>
       </c>
       <c r="J25" s="136"/>
       <c r="K25" s="135">
         <f>SUM(K12:K23)</f>
-        <v>7.4666666666666686</v>
+        <v>8.0166666666666675</v>
       </c>
       <c r="L25" s="229"/>
       <c r="M25" s="229"/>
@@ -41141,23 +41186,23 @@
       <c r="B26" s="53"/>
       <c r="C26" s="54">
         <f>C25/$K$25</f>
-        <v>0.14062500000000006</v>
+        <v>0.16839916839916855</v>
       </c>
       <c r="E26" s="54">
         <f>E25/$K$25</f>
-        <v>0.23660714285714218</v>
+        <v>0.2203742203742198</v>
       </c>
       <c r="G26" s="54">
         <f>G25/$K$25</f>
-        <v>0.32589285714285759</v>
+        <v>0.303534303534304</v>
       </c>
       <c r="I26" s="54">
         <f>I25/$K$25</f>
-        <v>0.29687500000000017</v>
+        <v>0.30769230769230788</v>
       </c>
       <c r="K26" s="55">
         <f>1-K25/24</f>
-        <v>0.68888888888888888</v>
+        <v>0.66597222222222219</v>
       </c>
       <c r="L26" s="229"/>
       <c r="M26" s="229"/>

</xml_diff>